<commit_message>
Documentatie inlezen gegevens + planning bijgewerkt
</commit_message>
<xml_diff>
--- a/documenten/kerntaak_1/1.4/ontwerpdocument/datadictionary/datadicionary.xlsx
+++ b/documenten/kerntaak_1/1.4/ontwerpdocument/datadictionary/datadicionary.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\did-you-had-a-good-day\documenten\kerntaak_1\1.4\datadictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\PvB\exam\documenten\kerntaak_1\1.4\ontwerpdocument\datadictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86942785-B0DF-4C80-AB83-B84CD072BDF3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15312" windowHeight="7560" xr2:uid="{D4BE1572-8E8D-4F40-9A5B-4DAAF23160B1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -72,9 +71,6 @@
     <t>hier komt een mail die de gebruiker heeft ingevult</t>
   </si>
   <si>
-    <t>passwoord</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aa.. Zz 1 .. 9 </t>
   </si>
   <si>
@@ -102,9 +98,6 @@
     <t>een automatisch gegenereerd nummer voor een nieuwe aangemaakte optie</t>
   </si>
   <si>
-    <t>hier komt automatic de datum wanneer er een nieuwe optie is aangemaakt</t>
-  </si>
-  <si>
     <t>optie</t>
   </si>
   <si>
@@ -157,12 +150,18 @@
   </si>
   <si>
     <t>hier komt een afbeelding die de gebruiker kan uploaden</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>hier komt automatisch de datum wanneer er een nieuwe optie is aangemaakt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -529,25 +528,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B13495-DD6B-481E-A2EC-BA0CB8262477}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,7 +564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -581,7 +581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -598,46 +598,46 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -662,55 +662,55 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>19</v>
-      </c>
-      <c r="C15" t="s">
-        <v>20</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -727,7 +727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -735,64 +735,64 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D22" t="s">
         <v>9</v>
       </c>
       <c r="E22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
         <v>32</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
         <v>33</v>
       </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>34</v>
-      </c>
-      <c r="D23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>36</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
       </c>
       <c r="E24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
         <v>41</v>
-      </c>
-      <c r="C25" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>